<commit_message>
have changed the compiler option and one stack 30min OK,many stacks 50min OK
</commit_message>
<xml_diff>
--- a/TC275C_OS/bug_fix_list.xlsx
+++ b/TC275C_OS/bug_fix_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Bug NO.</t>
   </si>
@@ -31,6 +31,9 @@
   <si>
     <t>delay() function is copied from TC1728 to TC275. the function can not work well because of the
 assembley updated</t>
+  </si>
+  <si>
+    <t>When the one stack mode is selected,  the trap below can be entered</t>
   </si>
 </sst>
 </file>
@@ -145,14 +148,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -171,6 +168,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,6 +192,87 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>74545</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>281608</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5912641</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1291132</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704023" y="2269434"/>
+          <a:ext cx="5838096" cy="1009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>99390</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1391480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5949465</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3105978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="728868" y="3379306"/>
+          <a:ext cx="5850075" cy="1714498"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -627,143 +714,147 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="84.5703125" customWidth="1"/>
+    <col min="2" max="2" width="114.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>42293</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>2</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>42328</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="3">
         <v>4</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="3">
         <v>5</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="3">
         <v>6</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="3">
         <v>7</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>8</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>9</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>10</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="3">
         <v>11</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="3">
         <v>12</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="3">
         <v>13</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="3">
         <v>14</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -771,6 +862,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>